<commit_message>
Monthly and income reports
</commit_message>
<xml_diff>
--- a/app/templates/report/ingresos.xlsx
+++ b/app/templates/report/ingresos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8D80D7-D6D6-4C2C-9923-921B45CACC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CAB75E-7641-457F-8C7D-DA4211BB42CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingresos!$A$3:$N$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingresos!$A$3:$P$3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Mes</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Ciente</t>
   </si>
   <si>
-    <t>Renta</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>Estado</t>
-  </si>
-  <si>
-    <t>Renta pendiente</t>
   </si>
   <si>
     <t>Check
@@ -97,6 +91,18 @@
   </si>
   <si>
     <t>Factura</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Importe</t>
+  </si>
+  <si>
+    <t>Importe pendiente</t>
+  </si>
+  <si>
+    <t>Renta o Servicio</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,6 +283,12 @@
     </xf>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -662,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -670,55 +682,60 @@
   <cols>
     <col min="1" max="1" width="39.42578125" style="9" customWidth="1"/>
     <col min="2" max="3" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.5703125" style="9" customWidth="1"/>
-    <col min="9" max="12" width="13.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.85546875" style="1"/>
+    <col min="4" max="4" width="9.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5703125" style="9" customWidth="1"/>
+    <col min="10" max="11" width="13.7109375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="19" customWidth="1"/>
+    <col min="13" max="14" width="13.7109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="11"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="13">
-        <f>I2*0.13</f>
+      <c r="H1" s="16"/>
+      <c r="I1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="13">
+        <f>J2*0.13</f>
         <v>0</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="13">
-        <f>SUBTOTAL(9,I4:I99999)</f>
+      <c r="H2" s="16"/>
+      <c r="I2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="13">
+        <f>SUBTOTAL(9,J4:J99999)</f>
         <v>0</v>
       </c>
-      <c r="J2" s="13">
-        <f t="shared" ref="J2:K2" si="0">SUBTOTAL(9,J4:J99999)</f>
+      <c r="K2" s="13">
+        <f t="shared" ref="K2" si="0">SUBTOTAL(9,K4:K99999)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
     </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>0</v>
@@ -727,63 +744,71 @@
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="P3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="3"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:N3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A3:P3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Tax & Management fee
</commit_message>
<xml_diff>
--- a/app/templates/report/ingresos.xlsx
+++ b/app/templates/report/ingresos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07dae84afc6a2e79/Development/projects/ciber/cotown/back/app/templates/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{F5CAB75E-7641-457F-8C7D-DA4211BB42CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F948220D-8B80-493E-B6C7-2955E501942D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E071F3C-81A3-4C23-A39F-A74408D9846A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ingresos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingresos!$A$2:$R$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingresos!$A$2:$T$2</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Mes</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Management Fee</t>
+  </si>
+  <si>
+    <t>Importe Neto</t>
+  </si>
+  <si>
+    <t>IVA</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,6 +166,10 @@
       <sz val="10"/>
       <name val="Century Gothic"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -228,12 +238,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -296,11 +307,15 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,10 +396,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -684,31 +695,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" style="9" customWidth="1"/>
-    <col min="2" max="3" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.5703125" style="9" customWidth="1"/>
-    <col min="10" max="11" width="13.85546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="19" customWidth="1"/>
-    <col min="15" max="16" width="13.7109375" style="7" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.85546875" style="1"/>
+    <col min="1" max="1" width="39.44140625" style="9" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.5546875" style="9" customWidth="1"/>
+    <col min="10" max="11" width="13.88671875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="6.77734375" style="7" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="5.5546875" style="7" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" style="7" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" style="19" customWidth="1"/>
+    <col min="17" max="18" width="13.6640625" style="7" customWidth="1"/>
+    <col min="19" max="19" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
@@ -726,15 +739,17 @@
         <v>0</v>
       </c>
       <c r="L1" s="14"/>
-      <c r="M1" s="13">
-        <f>SUBTOTAL(9,M3:M99998)</f>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="13">
+        <f>SUBTOTAL(9,O3:O99998)</f>
         <v>0</v>
       </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
     </row>
-    <row r="2" spans="1:18" s="4" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="25.2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -768,27 +783,33 @@
       <c r="K2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="15" t="s">
+      <c r="O2" s="20"/>
+      <c r="P2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -804,21 +825,26 @@
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="21"/>
+      <c r="L3" s="22"/>
       <c r="M3" s="8">
-        <f>J3*L3</f>
+        <f>J3/(1+L3)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="8">
+        <f>M3*N3</f>
+        <v>0</v>
+      </c>
       <c r="P3" s="17"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="5" t="s">
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:R2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:T2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>